<commit_message>
Modified 0.1s model run complete
</commit_message>
<xml_diff>
--- a/Graphs/AC_tank_conductivity_sweep_results.xlsx
+++ b/Graphs/AC_tank_conductivity_sweep_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="90" uniqueCount="9">
   <si>
     <t>Insulation equivalent conductivity (W/mK)</t>
   </si>
@@ -136,28 +136,28 @@
         <v>7.1428571428571427e-06</v>
       </c>
       <c r="B2" s="0">
-        <v>33.112855293953096</v>
+        <v>32.77329241352902</v>
       </c>
       <c r="C2" s="0">
-        <v>16.477536686903456</v>
+        <v>16.274835892552474</v>
       </c>
       <c r="D2" s="0">
-        <v>0.49761751261337167</v>
+        <v>0.49658837101865666</v>
       </c>
       <c r="E2" s="0">
-        <v>29.781359557209051</v>
+        <v>29.320677753896625</v>
       </c>
       <c r="F2" s="0">
-        <v>14.808362530511371</v>
+        <v>14.579297759489732</v>
       </c>
       <c r="G2" s="0">
-        <v>0.4972359472731584</v>
+        <v>0.49723604214954376</v>
       </c>
       <c r="H2" s="0">
-        <v>302.5</v>
+        <v>299.05770891393894</v>
       </c>
       <c r="I2" s="0">
-        <v>268</v>
+        <v>265.42554296131311</v>
       </c>
     </row>
     <row r="3">
@@ -165,28 +165,28 @@
         <v>1.5703744254353434e-05</v>
       </c>
       <c r="B3" s="0">
-        <v>33.115665233172315</v>
+        <v>32.774252026261962</v>
       </c>
       <c r="C3" s="0">
-        <v>16.485459357441894</v>
+        <v>16.275195457947795</v>
       </c>
       <c r="D3" s="0">
-        <v>0.497814531019242</v>
+        <v>0.49658480214610251</v>
       </c>
       <c r="E3" s="0">
-        <v>29.786072644022013</v>
+        <v>29.272639081544099</v>
       </c>
       <c r="F3" s="0">
-        <v>14.817389911801088</v>
+        <v>14.483270274595737</v>
       </c>
       <c r="G3" s="0">
-        <v>0.49746034292221131</v>
+        <v>0.49477159316760039</v>
       </c>
       <c r="H3" s="0">
-        <v>302.5</v>
+        <v>299</v>
       </c>
       <c r="I3" s="0">
-        <v>268</v>
+        <v>265.50939299472316</v>
       </c>
     </row>
     <row r="4">
@@ -194,28 +194,28 @@
         <v>3.4525061704859374e-05</v>
       </c>
       <c r="B4" s="0">
-        <v>33.111467294396569</v>
+        <v>32.772793603631591</v>
       </c>
       <c r="C4" s="0">
-        <v>16.468605511681957</v>
+        <v>16.275607717764231</v>
       </c>
       <c r="D4" s="0">
-        <v>0.4973686416629724</v>
+        <v>0.49661948000553457</v>
       </c>
       <c r="E4" s="0">
-        <v>29.781161594693586</v>
+        <v>29.316903451891847</v>
       </c>
       <c r="F4" s="0">
-        <v>14.804861553534153</v>
+        <v>14.524171121694941</v>
       </c>
       <c r="G4" s="0">
-        <v>0.49712169575588638</v>
+        <v>0.49541968665035402</v>
       </c>
       <c r="H4" s="0">
-        <v>302.5</v>
+        <v>299</v>
       </c>
       <c r="I4" s="0">
-        <v>268</v>
+        <v>265.68202053819147</v>
       </c>
     </row>
     <row r="5">
@@ -223,28 +223,28 @@
         <v>7.5904183513043625e-05</v>
       </c>
       <c r="B5" s="0">
-        <v>33.110233855326683</v>
+        <v>32.772481962142614</v>
       </c>
       <c r="C5" s="0">
-        <v>16.512279097439258</v>
+        <v>16.276321602329066</v>
       </c>
       <c r="D5" s="0">
-        <v>0.49870620574861352</v>
+        <v>0.49664598552928596</v>
       </c>
       <c r="E5" s="0">
-        <v>29.778592448089249</v>
+        <v>29.30691429262793</v>
       </c>
       <c r="F5" s="0">
-        <v>14.803771464498212</v>
+        <v>14.603291602409788</v>
       </c>
       <c r="G5" s="0">
-        <v>0.49712797843969619</v>
+        <v>0.49828826933455783</v>
       </c>
       <c r="H5" s="0">
-        <v>302.5</v>
+        <v>298.9497081585269</v>
       </c>
       <c r="I5" s="0">
-        <v>268</v>
+        <v>265.39255207683027</v>
       </c>
     </row>
     <row r="6">
@@ -252,28 +252,28 @@
         <v>0.00016687718400140863</v>
       </c>
       <c r="B6" s="0">
-        <v>33.107054179915011</v>
+        <v>32.769371324296081</v>
       </c>
       <c r="C6" s="0">
-        <v>16.473084792885352</v>
+        <v>16.280739717284661</v>
       </c>
       <c r="D6" s="0">
-        <v>0.49757023694602964</v>
+        <v>0.49682795425537163</v>
       </c>
       <c r="E6" s="0">
-        <v>29.762119657212772</v>
+        <v>29.297991960860699</v>
       </c>
       <c r="F6" s="0">
-        <v>14.785457341088614</v>
+        <v>14.547901135108079</v>
       </c>
       <c r="G6" s="0">
-        <v>0.49678777961318349</v>
+        <v>0.49654942750147096</v>
       </c>
       <c r="H6" s="0">
-        <v>302.5</v>
+        <v>299.07415270253398</v>
       </c>
       <c r="I6" s="0">
-        <v>268</v>
+        <v>265.36600548902254</v>
       </c>
     </row>
     <row r="7">
@@ -281,28 +281,28 @@
         <v>0.00036688352672227227</v>
       </c>
       <c r="B7" s="0">
-        <v>33.099329825652383</v>
+        <v>32.76122057453825</v>
       </c>
       <c r="C7" s="0">
-        <v>16.478742460347576</v>
+        <v>16.285613400966337</v>
       </c>
       <c r="D7" s="0">
-        <v>0.4978572843362028</v>
+        <v>0.49710032518212649</v>
       </c>
       <c r="E7" s="0">
-        <v>29.738937816373408</v>
+        <v>29.319446752684335</v>
       </c>
       <c r="F7" s="0">
-        <v>14.708452733508036</v>
+        <v>14.528667127739583</v>
       </c>
       <c r="G7" s="0">
-        <v>0.49458567835633938</v>
+        <v>0.49553005724466526</v>
       </c>
       <c r="H7" s="0">
-        <v>302.5</v>
+        <v>298.94012124375212</v>
       </c>
       <c r="I7" s="0">
-        <v>268.5</v>
+        <v>265.59005044578947</v>
       </c>
     </row>
     <row r="8">
@@ -310,28 +310,28 @@
         <v>0.00080660231046945235</v>
       </c>
       <c r="B8" s="0">
-        <v>33.08523539718076</v>
+        <v>32.794728442994554</v>
       </c>
       <c r="C8" s="0">
-        <v>16.49413134224752</v>
+        <v>16.298977203582815</v>
       </c>
       <c r="D8" s="0">
-        <v>0.49853450169657881</v>
+        <v>0.4969999136268049</v>
       </c>
       <c r="E8" s="0">
-        <v>29.89853309090423</v>
+        <v>29.400424879797164</v>
       </c>
       <c r="F8" s="0">
-        <v>14.789346489344034</v>
+        <v>14.528099914219124</v>
       </c>
       <c r="G8" s="0">
-        <v>0.4946512407273676</v>
+        <v>0.4941459170612964</v>
       </c>
       <c r="H8" s="0">
-        <v>302.5</v>
+        <v>299.04531566934696</v>
       </c>
       <c r="I8" s="0">
-        <v>269</v>
+        <v>266.0247110216535</v>
       </c>
     </row>
     <row r="9">
@@ -339,28 +339,28 @@
         <v>0.0017733346958016011</v>
       </c>
       <c r="B9" s="0">
-        <v>33.05280257048009</v>
+        <v>32.811284433865559</v>
       </c>
       <c r="C9" s="0">
-        <v>16.493550047465828</v>
+        <v>16.342171135941747</v>
       </c>
       <c r="D9" s="0">
-        <v>0.49900609826642789</v>
+        <v>0.49806557158349091</v>
       </c>
       <c r="E9" s="0">
-        <v>30.001801282348069</v>
+        <v>29.509394935202451</v>
       </c>
       <c r="F9" s="0">
-        <v>14.76990734241096</v>
+        <v>14.554407235259344</v>
       </c>
       <c r="G9" s="0">
-        <v>0.4923006856625311</v>
+        <v>0.49321266217820853</v>
       </c>
       <c r="H9" s="0">
-        <v>302.5</v>
+        <v>299.5</v>
       </c>
       <c r="I9" s="0">
-        <v>270</v>
+        <v>266.9838460207726</v>
       </c>
     </row>
     <row r="10">
@@ -368,28 +368,28 @@
         <v>0.0038987192356335991</v>
       </c>
       <c r="B10" s="0">
-        <v>33.237294438940467</v>
+        <v>32.883544459803936</v>
       </c>
       <c r="C10" s="0">
-        <v>16.649381482913075</v>
+        <v>16.376378724027308</v>
       </c>
       <c r="D10" s="0">
-        <v>0.50092469209548041</v>
+        <v>0.49801136079005731</v>
       </c>
       <c r="E10" s="0">
-        <v>30.178606413178485</v>
+        <v>29.773284346783221</v>
       </c>
       <c r="F10" s="0">
-        <v>14.823182440216005</v>
+        <v>14.574585052800272</v>
       </c>
       <c r="G10" s="0">
-        <v>0.49118180731310951</v>
+        <v>0.48951888824367962</v>
       </c>
       <c r="H10" s="0">
-        <v>303</v>
+        <v>299.52225066632963</v>
       </c>
       <c r="I10" s="0">
-        <v>272</v>
+        <v>268.96354852795059</v>
       </c>
     </row>
     <row r="11">
@@ -397,28 +397,28 @@
         <v>0.0085714285714285684</v>
       </c>
       <c r="B11" s="0">
-        <v>33.312460642886016</v>
+        <v>33.010550936512153</v>
       </c>
       <c r="C11" s="0">
-        <v>16.394763092104728</v>
+        <v>16.238632654447056</v>
       </c>
       <c r="D11" s="0">
-        <v>0.49215106827018146</v>
+        <v>0.49192249731542365</v>
       </c>
       <c r="E11" s="0">
-        <v>31.183773658018595</v>
+        <v>30.095801120460571</v>
       </c>
       <c r="F11" s="0">
-        <v>15.525855409672339</v>
+        <v>14.949946014553548</v>
       </c>
       <c r="G11" s="0">
-        <v>0.49788250709932985</v>
+        <v>0.49674524212581461</v>
       </c>
       <c r="H11" s="0">
-        <v>304</v>
+        <v>300.92703705314574</v>
       </c>
       <c r="I11" s="0">
-        <v>296</v>
+        <v>271.99088509064114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Successful run for 0.5s timestep
</commit_message>
<xml_diff>
--- a/Graphs/AC_tank_conductivity_sweep_results.xlsx
+++ b/Graphs/AC_tank_conductivity_sweep_results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="108" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="9" uniqueCount="9">
   <si>
     <t>Insulation equivalent conductivity (W/mK)</t>
   </si>
@@ -91,15 +91,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.53125" customWidth="true"/>
-    <col min="2" max="2" width="30.265625" customWidth="true"/>
-    <col min="3" max="3" width="28.86328125" customWidth="true"/>
-    <col min="4" max="4" width="35.19921875" customWidth="true"/>
-    <col min="5" max="5" width="29" customWidth="true"/>
-    <col min="6" max="6" width="27.59765625" customWidth="true"/>
-    <col min="7" max="7" width="33.9296875" customWidth="true"/>
-    <col min="8" max="8" width="29.19921875" customWidth="true"/>
-    <col min="9" max="9" width="27.9296875" customWidth="true"/>
+    <col min="1" max="1" width="38.7109375" customWidth="true"/>
+    <col min="2" max="2" width="33.28515625" customWidth="true"/>
+    <col min="3" max="3" width="31.85546875" customWidth="true"/>
+    <col min="4" max="4" width="38.7109375" customWidth="true"/>
+    <col min="5" max="5" width="32" customWidth="true"/>
+    <col min="6" max="6" width="30.5703125" customWidth="true"/>
+    <col min="7" max="7" width="37.42578125" customWidth="true"/>
+    <col min="8" max="8" width="32.28515625" customWidth="true"/>
+    <col min="9" max="9" width="31" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -136,28 +136,28 @@
         <v>7.1428571428571427e-06</v>
       </c>
       <c r="B2" s="0">
-        <v>34.988949577304084</v>
+        <v>33.39826164720219</v>
       </c>
       <c r="C2" s="0">
-        <v>17.856004523332114</v>
+        <v>16.38729150882072</v>
       </c>
       <c r="D2" s="0">
-        <v>0.51033268329137216</v>
+        <v>0.49066300761176002</v>
       </c>
       <c r="E2" s="0">
-        <v>31.246316170460439</v>
+        <v>30.215296610272709</v>
       </c>
       <c r="F2" s="0">
-        <v>15.491341858194986</v>
+        <v>15.079108844444091</v>
       </c>
       <c r="G2" s="0">
-        <v>0.49578138343361416</v>
+        <v>0.49905546316290139</v>
       </c>
       <c r="H2" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I2" s="0">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3">
@@ -165,28 +165,28 @@
         <v>1.5703744254353434e-05</v>
       </c>
       <c r="B3" s="0">
-        <v>35.00115014608722</v>
+        <v>33.393007005583534</v>
       </c>
       <c r="C3" s="0">
-        <v>17.813683658203843</v>
+        <v>16.376170279596163</v>
       </c>
       <c r="D3" s="0">
-        <v>0.50894566560965526</v>
+        <v>0.49040717647434262</v>
       </c>
       <c r="E3" s="0">
-        <v>31.26699230314231</v>
+        <v>30.227659038314179</v>
       </c>
       <c r="F3" s="0">
-        <v>15.508784075076013</v>
+        <v>15.093070195559724</v>
       </c>
       <c r="G3" s="0">
-        <v>0.49601138237774767</v>
+        <v>0.49931323416176382</v>
       </c>
       <c r="H3" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I3" s="0">
-        <v>237</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4">
@@ -194,28 +194,28 @@
         <v>3.4525061704859374e-05</v>
       </c>
       <c r="B4" s="0">
-        <v>34.97401099412528</v>
+        <v>33.394175241246103</v>
       </c>
       <c r="C4" s="0">
-        <v>17.840200087432933</v>
+        <v>16.381286253180967</v>
       </c>
       <c r="D4" s="0">
-        <v>0.5100987727838715</v>
+        <v>0.49054322003281492</v>
       </c>
       <c r="E4" s="0">
-        <v>31.239117956781932</v>
+        <v>30.598308210939202</v>
       </c>
       <c r="F4" s="0">
-        <v>15.491780214759956</v>
+        <v>15.423707379763925</v>
       </c>
       <c r="G4" s="0">
-        <v>0.49590965520192387</v>
+        <v>0.50407059349280614</v>
       </c>
       <c r="H4" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I4" s="0">
-        <v>237</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="5">
@@ -223,28 +223,28 @@
         <v>7.5904183513043625e-05</v>
       </c>
       <c r="B5" s="0">
-        <v>34.998955165654969</v>
+        <v>33.398601568318696</v>
       </c>
       <c r="C5" s="0">
-        <v>17.81910465664971</v>
+        <v>16.390294869607398</v>
       </c>
       <c r="D5" s="0">
-        <v>0.50913247473558532</v>
+        <v>0.49074793853509524</v>
       </c>
       <c r="E5" s="0">
-        <v>31.277388641370884</v>
+        <v>30.611375710962818</v>
       </c>
       <c r="F5" s="0">
-        <v>15.532217654842968</v>
+        <v>15.442872311903681</v>
       </c>
       <c r="G5" s="0">
-        <v>0.49659573031932608</v>
+        <v>0.50448148615461086</v>
       </c>
       <c r="H5" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I5" s="0">
-        <v>237</v>
+        <v>246.5</v>
       </c>
     </row>
     <row r="6">
@@ -252,28 +252,28 @@
         <v>0.00016687718400140863</v>
       </c>
       <c r="B6" s="0">
-        <v>34.974807443003286</v>
+        <v>33.395289403448629</v>
       </c>
       <c r="C6" s="0">
-        <v>17.802497516244781</v>
+        <v>16.398530720110681</v>
       </c>
       <c r="D6" s="0">
-        <v>0.50900916453240319</v>
+        <v>0.49104322834277503</v>
       </c>
       <c r="E6" s="0">
-        <v>31.234555628178178</v>
+        <v>30.577859917344405</v>
       </c>
       <c r="F6" s="0">
-        <v>15.493205081226979</v>
+        <v>15.411304350065533</v>
       </c>
       <c r="G6" s="0">
-        <v>0.49602770936333801</v>
+        <v>0.50400205873544202</v>
       </c>
       <c r="H6" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I6" s="0">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7">
@@ -281,28 +281,28 @@
         <v>0.00036688352672227227</v>
       </c>
       <c r="B7" s="0">
-        <v>34.979855434960754</v>
+        <v>33.396246319244682</v>
       </c>
       <c r="C7" s="0">
-        <v>17.780588788830105</v>
+        <v>16.362092454254388</v>
       </c>
       <c r="D7" s="0">
-        <v>0.50830938457965225</v>
+        <v>0.48993806962148573</v>
       </c>
       <c r="E7" s="0">
-        <v>31.217414912278393</v>
+        <v>30.585039333651231</v>
       </c>
       <c r="F7" s="0">
-        <v>15.47369814692432</v>
+        <v>15.436554357075178</v>
       </c>
       <c r="G7" s="0">
-        <v>0.49567519252973846</v>
+        <v>0.50470931845724609</v>
       </c>
       <c r="H7" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I7" s="0">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8">
@@ -310,28 +310,28 @@
         <v>0.00080660231046945235</v>
       </c>
       <c r="B8" s="0">
-        <v>34.936832399688306</v>
+        <v>33.393850875056195</v>
       </c>
       <c r="C8" s="0">
-        <v>17.710416884521276</v>
+        <v>16.292657773193024</v>
       </c>
       <c r="D8" s="0">
-        <v>0.50692680669811618</v>
+        <v>0.48789394892348148</v>
       </c>
       <c r="E8" s="0">
-        <v>31.166949057456016</v>
+        <v>30.560629894508651</v>
       </c>
       <c r="F8" s="0">
-        <v>15.457345884579231</v>
+        <v>15.460669159829573</v>
       </c>
       <c r="G8" s="0">
-        <v>0.49595312829894711</v>
+        <v>0.50590152144107658</v>
       </c>
       <c r="H8" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I8" s="0">
-        <v>237</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9">
@@ -339,28 +339,28 @@
         <v>0.0017733346958016011</v>
       </c>
       <c r="B9" s="0">
-        <v>34.869611819251347</v>
+        <v>33.392833487079926</v>
       </c>
       <c r="C9" s="0">
-        <v>17.555737078289653</v>
+        <v>16.391326996350344</v>
       </c>
       <c r="D9" s="0">
-        <v>0.50346809621199207</v>
+        <v>0.49086361607176399</v>
       </c>
       <c r="E9" s="0">
-        <v>31.045808804183494</v>
+        <v>30.495955758681198</v>
       </c>
       <c r="F9" s="0">
-        <v>15.365550345431465</v>
+        <v>15.513662856708413</v>
       </c>
       <c r="G9" s="0">
-        <v>0.49493155235050351</v>
+        <v>0.50871213807726556</v>
       </c>
       <c r="H9" s="0">
-        <v>329</v>
+        <v>281.5</v>
       </c>
       <c r="I9" s="0">
-        <v>238</v>
+        <v>247.5</v>
       </c>
     </row>
     <row r="10">
@@ -368,28 +368,28 @@
         <v>0.0038987192356335991</v>
       </c>
       <c r="B10" s="0">
-        <v>34.707138475247675</v>
+        <v>33.379616736788194</v>
       </c>
       <c r="C10" s="0">
-        <v>17.175361327757447</v>
+        <v>16.586822353690732</v>
       </c>
       <c r="D10" s="0">
-        <v>0.49486538165647148</v>
+        <v>0.49691470349958022</v>
       </c>
       <c r="E10" s="0">
-        <v>32.061893206456823</v>
+        <v>30.65954788278497</v>
       </c>
       <c r="F10" s="0">
-        <v>16.769636624416197</v>
+        <v>15.848681860213294</v>
       </c>
       <c r="G10" s="0">
-        <v>0.52303950101858065</v>
+        <v>0.51692483923131072</v>
       </c>
       <c r="H10" s="0">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="I10" s="0">
-        <v>262</v>
+        <v>248.5</v>
       </c>
     </row>
     <row r="11">
@@ -397,28 +397,28 @@
         <v>0.0085714285714285684</v>
       </c>
       <c r="B11" s="0">
-        <v>33.010550936512153</v>
+        <v>33.366263791917689</v>
       </c>
       <c r="C11" s="0">
-        <v>16.238632654447056</v>
+        <v>17.04658192622751</v>
       </c>
       <c r="D11" s="0">
-        <v>0.49192249731542365</v>
+        <v>0.51089273982053407</v>
       </c>
       <c r="E11" s="0">
-        <v>30.095801120460571</v>
+        <v>30.804118776779305</v>
       </c>
       <c r="F11" s="0">
-        <v>14.949946014553548</v>
+        <v>16.34586317294519</v>
       </c>
       <c r="G11" s="0">
-        <v>0.49674524212581461</v>
+        <v>0.53063888278690163</v>
       </c>
       <c r="H11" s="0">
-        <v>300.92703705314574</v>
+        <v>282</v>
       </c>
       <c r="I11" s="0">
-        <v>271.99088509064114</v>
+        <v>271.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed valve smoothing ratio, increased stability
</commit_message>
<xml_diff>
--- a/Graphs/AC_tank_conductivity_sweep_results.xlsx
+++ b/Graphs/AC_tank_conductivity_sweep_results.xlsx
@@ -136,28 +136,28 @@
         <v>7.1428571428571427e-06</v>
       </c>
       <c r="B2" s="0">
-        <v>33.39826164720219</v>
+        <v>34.913776369470838</v>
       </c>
       <c r="C2" s="0">
-        <v>16.38729150882072</v>
+        <v>16.046616270646645</v>
       </c>
       <c r="D2" s="0">
-        <v>0.49066300761176002</v>
+        <v>0.45960700729807219</v>
       </c>
       <c r="E2" s="0">
-        <v>30.215296610272709</v>
+        <v>30.658450542146987</v>
       </c>
       <c r="F2" s="0">
-        <v>15.079108844444091</v>
+        <v>15.259614157230043</v>
       </c>
       <c r="G2" s="0">
-        <v>0.49905546316290139</v>
+        <v>0.49772946405925655</v>
       </c>
       <c r="H2" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I2" s="0">
-        <v>246</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3">
@@ -165,28 +165,28 @@
         <v>1.5703744254353434e-05</v>
       </c>
       <c r="B3" s="0">
-        <v>33.393007005583534</v>
+        <v>34.922945321561237</v>
       </c>
       <c r="C3" s="0">
-        <v>16.376170279596163</v>
+        <v>16.057267664509535</v>
       </c>
       <c r="D3" s="0">
-        <v>0.49040717647434262</v>
+        <v>0.45979133537158634</v>
       </c>
       <c r="E3" s="0">
-        <v>30.227659038314179</v>
+        <v>30.660296317883805</v>
       </c>
       <c r="F3" s="0">
-        <v>15.093070195559724</v>
+        <v>15.260272694877289</v>
       </c>
       <c r="G3" s="0">
-        <v>0.49931323416176382</v>
+        <v>0.49772097884051247</v>
       </c>
       <c r="H3" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I3" s="0">
-        <v>246</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4">
@@ -194,28 +194,28 @@
         <v>3.4525061704859374e-05</v>
       </c>
       <c r="B4" s="0">
-        <v>33.394175241246103</v>
+        <v>34.907910898952814</v>
       </c>
       <c r="C4" s="0">
-        <v>16.381286253180967</v>
+        <v>16.043983620324116</v>
       </c>
       <c r="D4" s="0">
-        <v>0.49054322003281492</v>
+        <v>0.45960881665953296</v>
       </c>
       <c r="E4" s="0">
-        <v>30.598308210939202</v>
+        <v>30.655801210163922</v>
       </c>
       <c r="F4" s="0">
-        <v>15.423707379763925</v>
+        <v>15.266772246831055</v>
       </c>
       <c r="G4" s="0">
-        <v>0.50407059349280614</v>
+        <v>0.49800597747121877</v>
       </c>
       <c r="H4" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I4" s="0">
-        <v>246.5</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
@@ -223,28 +223,28 @@
         <v>7.5904183513043625e-05</v>
       </c>
       <c r="B5" s="0">
-        <v>33.398601568318696</v>
+        <v>34.905703523018794</v>
       </c>
       <c r="C5" s="0">
-        <v>16.390294869607398</v>
+        <v>16.045393555512156</v>
       </c>
       <c r="D5" s="0">
-        <v>0.49074793853509524</v>
+        <v>0.45967827420899615</v>
       </c>
       <c r="E5" s="0">
-        <v>30.611375710962818</v>
+        <v>30.647876950116746</v>
       </c>
       <c r="F5" s="0">
-        <v>15.442872311903681</v>
+        <v>15.241345824614058</v>
       </c>
       <c r="G5" s="0">
-        <v>0.50448148615461086</v>
+        <v>0.4973051102176263</v>
       </c>
       <c r="H5" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I5" s="0">
-        <v>246.5</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6">
@@ -252,28 +252,28 @@
         <v>0.00016687718400140863</v>
       </c>
       <c r="B6" s="0">
-        <v>33.395289403448629</v>
+        <v>34.917519062778261</v>
       </c>
       <c r="C6" s="0">
-        <v>16.398530720110681</v>
+        <v>16.066660234786756</v>
       </c>
       <c r="D6" s="0">
-        <v>0.49104322834277503</v>
+        <v>0.46013178100942631</v>
       </c>
       <c r="E6" s="0">
-        <v>30.577859917344405</v>
+        <v>30.636079126776572</v>
       </c>
       <c r="F6" s="0">
-        <v>15.411304350065533</v>
+        <v>15.252227690426082</v>
       </c>
       <c r="G6" s="0">
-        <v>0.50400205873544202</v>
+        <v>0.49785181802508521</v>
       </c>
       <c r="H6" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I6" s="0">
-        <v>247</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7">
@@ -281,28 +281,28 @@
         <v>0.00036688352672227227</v>
       </c>
       <c r="B7" s="0">
-        <v>33.396246319244682</v>
+        <v>34.901535472372629</v>
       </c>
       <c r="C7" s="0">
-        <v>16.362092454254388</v>
+        <v>16.0713571228364</v>
       </c>
       <c r="D7" s="0">
-        <v>0.48993806962148573</v>
+        <v>0.4604770794556638</v>
       </c>
       <c r="E7" s="0">
-        <v>30.585039333651231</v>
+        <v>30.965267588605251</v>
       </c>
       <c r="F7" s="0">
-        <v>15.436554357075178</v>
+        <v>15.541494007393675</v>
       </c>
       <c r="G7" s="0">
-        <v>0.50470931845724609</v>
+        <v>0.50190084626017284</v>
       </c>
       <c r="H7" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I7" s="0">
-        <v>247</v>
+        <v>302</v>
       </c>
     </row>
     <row r="8">
@@ -310,28 +310,28 @@
         <v>0.00080660231046945235</v>
       </c>
       <c r="B8" s="0">
-        <v>33.393850875056195</v>
+        <v>34.887273081492978</v>
       </c>
       <c r="C8" s="0">
-        <v>16.292657773193024</v>
+        <v>16.104782033631658</v>
       </c>
       <c r="D8" s="0">
-        <v>0.48789394892348148</v>
+        <v>0.46162341195348205</v>
       </c>
       <c r="E8" s="0">
-        <v>30.560629894508651</v>
+        <v>30.912421485517669</v>
       </c>
       <c r="F8" s="0">
-        <v>15.460669159829573</v>
+        <v>15.537837079453327</v>
       </c>
       <c r="G8" s="0">
-        <v>0.50590152144107658</v>
+        <v>0.50264056753796316</v>
       </c>
       <c r="H8" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I8" s="0">
-        <v>247</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9">
@@ -339,28 +339,28 @@
         <v>0.0017733346958016011</v>
       </c>
       <c r="B9" s="0">
-        <v>33.392833487079926</v>
+        <v>34.851684462076136</v>
       </c>
       <c r="C9" s="0">
-        <v>16.391326996350344</v>
+        <v>16.170131056300125</v>
       </c>
       <c r="D9" s="0">
-        <v>0.49086361607176399</v>
+        <v>0.46396985700635662</v>
       </c>
       <c r="E9" s="0">
-        <v>30.495955758681198</v>
+        <v>30.763331295120999</v>
       </c>
       <c r="F9" s="0">
-        <v>15.513662856708413</v>
+        <v>15.463066326108835</v>
       </c>
       <c r="G9" s="0">
-        <v>0.50871213807726556</v>
+        <v>0.50264602938373082</v>
       </c>
       <c r="H9" s="0">
-        <v>281.5</v>
+        <v>338.5</v>
       </c>
       <c r="I9" s="0">
-        <v>247.5</v>
+        <v>302.5</v>
       </c>
     </row>
     <row r="10">
@@ -368,28 +368,28 @@
         <v>0.0038987192356335991</v>
       </c>
       <c r="B10" s="0">
-        <v>33.379616736788194</v>
+        <v>35.267866443531076</v>
       </c>
       <c r="C10" s="0">
-        <v>16.586822353690732</v>
+        <v>16.763699684893659</v>
       </c>
       <c r="D10" s="0">
-        <v>0.49691470349958022</v>
+        <v>0.47532503027181278</v>
       </c>
       <c r="E10" s="0">
-        <v>30.65954788278497</v>
+        <v>31.193345126036419</v>
       </c>
       <c r="F10" s="0">
-        <v>15.848681860213294</v>
+        <v>16.069243005674345</v>
       </c>
       <c r="G10" s="0">
-        <v>0.51692483923131072</v>
+        <v>0.51514971994015768</v>
       </c>
       <c r="H10" s="0">
-        <v>282</v>
+        <v>339</v>
       </c>
       <c r="I10" s="0">
-        <v>248.5</v>
+        <v>304.5</v>
       </c>
     </row>
     <row r="11">
@@ -397,28 +397,28 @@
         <v>0.0085714285714285684</v>
       </c>
       <c r="B11" s="0">
-        <v>33.366263791917689</v>
+        <v>35.115137281107216</v>
       </c>
       <c r="C11" s="0">
-        <v>17.04658192622751</v>
+        <v>17.18384179534123</v>
       </c>
       <c r="D11" s="0">
-        <v>0.51089273982053407</v>
+        <v>0.48935710140556815</v>
       </c>
       <c r="E11" s="0">
-        <v>30.804118776779305</v>
+        <v>31.782345969065368</v>
       </c>
       <c r="F11" s="0">
-        <v>16.34586317294519</v>
+        <v>16.801429943956588</v>
       </c>
       <c r="G11" s="0">
-        <v>0.53063888278690163</v>
+        <v>0.52864033260193832</v>
       </c>
       <c r="H11" s="0">
-        <v>282</v>
+        <v>339</v>
       </c>
       <c r="I11" s="0">
-        <v>271.5</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All nice graphs added
</commit_message>
<xml_diff>
--- a/Graphs/AC_tank_conductivity_sweep_results.xlsx
+++ b/Graphs/AC_tank_conductivity_sweep_results.xlsx
@@ -91,15 +91,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" customWidth="true"/>
-    <col min="2" max="2" width="33.28515625" customWidth="true"/>
-    <col min="3" max="3" width="31.85546875" customWidth="true"/>
-    <col min="4" max="4" width="38.7109375" customWidth="true"/>
-    <col min="5" max="5" width="32" customWidth="true"/>
-    <col min="6" max="6" width="30.5703125" customWidth="true"/>
-    <col min="7" max="7" width="37.42578125" customWidth="true"/>
-    <col min="8" max="8" width="32.28515625" customWidth="true"/>
-    <col min="9" max="9" width="31" customWidth="true"/>
+    <col min="1" max="1" width="34.53125" customWidth="true"/>
+    <col min="2" max="2" width="30.265625" customWidth="true"/>
+    <col min="3" max="3" width="28.86328125" customWidth="true"/>
+    <col min="4" max="4" width="35.19921875" customWidth="true"/>
+    <col min="5" max="5" width="29" customWidth="true"/>
+    <col min="6" max="6" width="27.59765625" customWidth="true"/>
+    <col min="7" max="7" width="33.9296875" customWidth="true"/>
+    <col min="8" max="8" width="29.19921875" customWidth="true"/>
+    <col min="9" max="9" width="27.9296875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>